<commit_message>
angepasst für Presetfunktion per Typ
</commit_message>
<xml_diff>
--- a/created_leaders_log.xlsx
+++ b/created_leaders_log.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F29"/>
+  <dimension ref="A1:F61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1349,6 +1349,1030 @@
         </is>
       </c>
     </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>2025-08-21T07:22:57</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Haus_B.3dm</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>0525f66e-fe44-413e-a4d2-beb390edd8e8</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>zargentuere</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>Standard 1:10 Zargenbeschriftung</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>zargentuere.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>2025-08-21T07:23:34</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Haus_B.3dm</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>12bb73f7-d6f1-4f90-b9c4-d824137b5ca1</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>zargentuere</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>Standard 1:10 Zargenbeschriftung</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>zargentuere.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>2025-08-21T07:24:10</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Haus_B.3dm</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>7de5608d-38d2-4592-9d92-4ee321e99e57</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>zargentuere</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>Standard 1:10 Zargenbeschriftung</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>zargentuere.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>2025-08-21T07:25:40</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Haus_B.3dm</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>436612dc-8e28-42e1-b7b9-9d8ddd7d1723</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>zargentuere</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>Standard 1:10 Zargenbeschriftung</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>zargentuere.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>2025-08-21T07:25:55</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Haus_B.3dm</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>8c65d0d3-12f6-47bb-ad27-374236345c7f</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>zargentuere</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>Standard 1:10 Zargenbeschriftung</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>zargentuere.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>2025-08-21T07:26:36</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Haus_B.3dm</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>a24634b9-c311-4fd4-a90b-2056fbd59603</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>rahmentuere_w</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>Standard 1:10 Rahmenbeschriftung WHG Eingang</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>rahmentuerew.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>2025-08-21T07:27:17</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Haus_B.3dm</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>a4942db9-b96b-4091-9a84-fc7a398957ad</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>rahmentuere_w</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>Standard 1:10 Rahmenbeschriftung WHG Eingang</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>rahmentuerew.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>2025-08-21T07:28:05</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Haus_B.3dm</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>c3a4f394-8a16-4450-a9ce-e7ea79494d13</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>rahmentuere_w</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>Standard 1:10 Rahmenbeschriftung WHG Eingang</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>rahmentuerew.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>2025-08-21T07:28:30</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Haus_B.3dm</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>9dd27323-a1cb-4594-bfd8-82b762ca7d4f</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>rahmentuere</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>Standard 1:10 Rahmenbeschriftung</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>rahmentuere.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>2025-08-21T07:34:57</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Haus_B.3dm</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>5ec54a75-e768-424a-929d-08a6a2f585d9</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>rahmentuere</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>Standard 1:10 Rahmenbeschriftung</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>rahmentuere.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>2025-08-21T07:35:55</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Haus_B.3dm</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>0c0c8aa3-cdc9-4cbc-a3c8-16510966b3b9</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>zargentuere</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>Standard 1:10 Zargenbeschriftung</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>zargentuere.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>2025-08-21T07:36:42</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Haus_B.3dm</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>31ef67a2-3823-4328-a160-fa8fb78b95b9</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>zargentuere</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>Standard 1:10 Zargenbeschriftung</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>zargentuere.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>2025-08-21T07:37:26</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>Haus_B.3dm</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>0ef27e03-7055-4f17-a320-3787d17657b8</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>zargentuere</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>Standard 1:10 Zargenbeschriftung</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>zargentuere.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>2025-08-21T07:37:48</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>Haus_B.3dm</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>f22e8e25-09db-4697-936f-ed849427c2f6</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>zargentuere</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>Standard 1:10 Zargenbeschriftung</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>zargentuere.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>2025-08-21T07:38:19</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>Haus_B.3dm</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>78f4d977-3f50-4d89-9526-85cbbdefb145</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>zargentuere</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>Standard 1:10 Zargenbeschriftung</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>zargentuere.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>2025-08-21T07:38:45</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>Haus_B.3dm</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>b870949e-ab73-4dc5-8cd6-a190aa69b45f</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>zargentuere</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>Standard 1:10 Zargenbeschriftung</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>zargentuere.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>2025-08-21T07:39:09</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>Haus_B.3dm</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>e9743612-ad46-41d9-807d-843f5efff1e1</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>zargentuere</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>Standard 1:10 Zargenbeschriftung</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>zargentuere.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>2025-08-21T07:39:31</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>Haus_B.3dm</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>afeb0386-c654-46b3-b397-b978512f1737</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>zargentuere</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>Standard 1:10 Zargenbeschriftung</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>zargentuere.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>2025-08-21T07:41:08</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>Haus_B.3dm</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>64d94098-810c-4b12-88bd-10c1e198a48d</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>schiebetuere</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>Standard 1:10 Schiebetürbeschriftung</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>schiebetuere.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>2025-08-21T07:41:37</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>Haus_B.3dm</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>7e039f2e-35fe-4dbd-8e09-06ff49750665</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>schiebetuere</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>Standard 1:10 Schiebetürbeschriftung</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>schiebetuere.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>2025-08-21T15:20:04</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>Haus_A.3dm</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>1c202ef5-3c9c-4e35-a924-d2ae95d019ab</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>zargentuere</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>Standard 1:10 Zargenbeschriftung</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>zargentuere.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>2025-08-21T15:33:31</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>Haus_A.3dm</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>a9760fd2-627e-45ab-bbcc-54109be14cc5</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>schiebetuere</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>Standard 1:10 Schiebetürbeschriftung</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>schiebetuere.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>2025-08-21T15:34:37</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>Haus_A.3dm</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>ef395ba8-6040-4c51-8d1e-eb597ff5158b</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>spez</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>Standard 1:10 Spez.Rahmenbeschriftung</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>spez.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>2025-08-21T15:40:32</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>Haus_A.3dm</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>92869a40-4619-440f-b718-352db991f927</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>zargentuere</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>Standard 1:10 Zargenbeschriftung</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>zargentuere.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>2025-08-21T16:10:20</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>Haus_D_test.3dm</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>7258b958-748a-4a7a-b9dc-fb1dc1284e61</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>zargentuere</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>Standard 1:10 Zargenbeschriftung</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>zargentuere.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>2025-08-21T16:29:06</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>Haus_D_test.3dm</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>12305b9a-7c5e-4a5c-81bc-9016e3fdd0d0</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>zargentuere</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>Standard 1:10 Zargenbeschriftung</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>zargentuere_2.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>2025-08-21T16:34:27</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>Haus_D_test.3dm</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>6f11d915-9e6a-4c02-90a2-a8ff763f6018</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>zargentuere</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>Standard 1:10 Zargenbeschriftung</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>zargentuere_2.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>2025-08-21T16:35:05</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>Haus_D_test.3dm</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>abf55ca4-1ec3-4367-b8af-491d9cc13913</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>zargentuere</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>Standard 1:10 Zargenbeschriftung</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>zargentuere.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>2025-08-21T16:35:22</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>Haus_D_test.3dm</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>d8cc6915-2784-4c94-bb37-c6945dc6e50f</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>rahmentuere</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>Standard 1:10 Rahmenbeschriftung</t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>rahmentuere.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>2025-08-21T16:39:10</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>Haus_D_test.3dm</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>c93fd141-acf6-49a1-9aa0-9cffd06b00ec</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>zargentuere</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>Standard 1:10 Zargenbeschriftung</t>
+        </is>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>zargentuere_2.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>2025-08-21T16:40:39</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>Haus_D_test.3dm</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>86a7fca8-f4f1-4248-ac47-aa6359fc762c</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>rahmentuere</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>Standard 1:10 Rahmenbeschriftung</t>
+        </is>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>rahmentuere.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>2025-08-21T16:52:59</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>Haus_D_test.3dm</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>96587c5c-6bcf-4357-80ad-b6b43e7414b1</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>zargentuere</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>Standard 1:10 Zargenbeschriftung</t>
+        </is>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>zargentuere_2.csv</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
diverse Erweiterungen der csv
</commit_message>
<xml_diff>
--- a/created_leaders_log.xlsx
+++ b/created_leaders_log.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F86"/>
+  <dimension ref="A1:F171"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3173,6 +3173,2726 @@
         </is>
       </c>
     </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>2025-09-02T11:43:45</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>Haus_C.3dm</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>d8d38571-b26d-4572-a372-bff11e4415e1</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>rahmentuere_w</t>
+        </is>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>Standard 1:10 Rahmenbeschriftung WHG Eingang</t>
+        </is>
+      </c>
+      <c r="F87" t="inlineStr">
+        <is>
+          <t>rahmentuerew.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>2025-09-02T11:44:50</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>Haus_C.3dm</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>d6d4cbc8-ddc6-4ac0-b19f-02df0ec89a59</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>zargentuere</t>
+        </is>
+      </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>Standard 1:10 Zargenbeschriftung</t>
+        </is>
+      </c>
+      <c r="F88" t="inlineStr">
+        <is>
+          <t>zargentuere.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>2025-09-02T11:45:45</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>Haus_C.3dm</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>72091ad8-32b4-469c-95d9-008572452593</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>zargentuere</t>
+        </is>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>Standard 1:10 Zargenbeschriftung</t>
+        </is>
+      </c>
+      <c r="F89" t="inlineStr">
+        <is>
+          <t>zargentuere.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>2025-09-02T11:46:26</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>Haus_C.3dm</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>96607c7a-4582-4235-9df4-a2db3d0221ed</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>zargentuere</t>
+        </is>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>Standard 1:10 Zargenbeschriftung</t>
+        </is>
+      </c>
+      <c r="F90" t="inlineStr">
+        <is>
+          <t>zargentuere.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>2025-09-02T11:46:52</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>Haus_C.3dm</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>35b2e396-dcf5-4720-b686-67860b516680</t>
+        </is>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>zargentuere</t>
+        </is>
+      </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>Standard 1:10 Zargenbeschriftung</t>
+        </is>
+      </c>
+      <c r="F91" t="inlineStr">
+        <is>
+          <t>zargentuere.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>2025-09-02T11:48:00</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>Haus_C.3dm</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>426971cf-56a5-4842-83db-4e0f935996c6</t>
+        </is>
+      </c>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>zargentuere</t>
+        </is>
+      </c>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>Standard 1:10 Zargenbeschriftung</t>
+        </is>
+      </c>
+      <c r="F92" t="inlineStr">
+        <is>
+          <t>zargentuere.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>2025-09-02T11:48:56</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>Haus_C.3dm</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>a6f5af47-fefe-443a-8eed-4e0692fabc8b</t>
+        </is>
+      </c>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t>zargentuere</t>
+        </is>
+      </c>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>Standard 1:10 Zargenbeschriftung</t>
+        </is>
+      </c>
+      <c r="F93" t="inlineStr">
+        <is>
+          <t>zargentuere.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>2025-09-02T11:49:59</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>Haus_C.3dm</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>df93c681-61f2-4bdf-a091-bb9825d4d1ad</t>
+        </is>
+      </c>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>rahmentuere</t>
+        </is>
+      </c>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>Standard 1:10 Rahmenbeschriftung</t>
+        </is>
+      </c>
+      <c r="F94" t="inlineStr">
+        <is>
+          <t>rahmentuere_nebenraum_Typ1.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>2025-09-02T12:04:19</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>Haus_C.3dm</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>cf4061cf-147a-4abb-9baf-2f144b0b0ff7</t>
+        </is>
+      </c>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>zargentuere</t>
+        </is>
+      </c>
+      <c r="E95" t="inlineStr">
+        <is>
+          <t>Standard 1:10 Zargenbeschriftung</t>
+        </is>
+      </c>
+      <c r="F95" t="inlineStr">
+        <is>
+          <t>zargentuere_Keller_EI30.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>2025-09-02T13:01:20</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>Haus_C.3dm</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>f7cc37ff-8bee-4dfe-9588-f8900754388b</t>
+        </is>
+      </c>
+      <c r="D96" t="inlineStr">
+        <is>
+          <t>zargentuere</t>
+        </is>
+      </c>
+      <c r="E96" t="inlineStr">
+        <is>
+          <t>Standard 1:10 Zargenbeschriftung</t>
+        </is>
+      </c>
+      <c r="F96" t="inlineStr">
+        <is>
+          <t>zargentuere_Keller_EI30.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>2025-09-02T13:03:17</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>Haus_C.3dm</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>421d1f23-94fd-4e6e-801f-965e6bd850db</t>
+        </is>
+      </c>
+      <c r="D97" t="inlineStr">
+        <is>
+          <t>rahmentuere</t>
+        </is>
+      </c>
+      <c r="E97" t="inlineStr">
+        <is>
+          <t>Standard 1:10 Rahmenbeschriftung</t>
+        </is>
+      </c>
+      <c r="F97" t="inlineStr">
+        <is>
+          <t>rahmentuere_nebenraum_Typ1.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>2025-09-02T13:16:52</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>Haus_C.3dm</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>5bcf33c7-8cd7-4d71-a5c4-fe0888ae27fd</t>
+        </is>
+      </c>
+      <c r="D98" t="inlineStr">
+        <is>
+          <t>zargentuere</t>
+        </is>
+      </c>
+      <c r="E98" t="inlineStr">
+        <is>
+          <t>Standard 1:10 Zargenbeschriftung</t>
+        </is>
+      </c>
+      <c r="F98" t="inlineStr">
+        <is>
+          <t>zargentuere.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>2025-09-02T13:22:13</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>Haus_C.3dm</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>bd0e26cc-f2d1-43f7-9834-710d21171232</t>
+        </is>
+      </c>
+      <c r="D99" t="inlineStr">
+        <is>
+          <t>zargentuere</t>
+        </is>
+      </c>
+      <c r="E99" t="inlineStr">
+        <is>
+          <t>Standard 1:10 Zargenbeschriftung</t>
+        </is>
+      </c>
+      <c r="F99" t="inlineStr">
+        <is>
+          <t>zargentuere_Keller_KK2B.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>2025-09-02T13:25:30</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>Haus_C.3dm</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>2dfb83a3-c120-4e30-b9f5-c4ef67b7c9a1</t>
+        </is>
+      </c>
+      <c r="D100" t="inlineStr">
+        <is>
+          <t>zargentuere</t>
+        </is>
+      </c>
+      <c r="E100" t="inlineStr">
+        <is>
+          <t>Standard 1:10 Zargenbeschriftung</t>
+        </is>
+      </c>
+      <c r="F100" t="inlineStr">
+        <is>
+          <t>zargentuere.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>2025-09-02T13:26:53</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>Haus_C.3dm</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>c99ac71f-5663-4889-afb1-cdedcd511cde</t>
+        </is>
+      </c>
+      <c r="D101" t="inlineStr">
+        <is>
+          <t>rahmentuere</t>
+        </is>
+      </c>
+      <c r="E101" t="inlineStr">
+        <is>
+          <t>Standard 1:10 Rahmenbeschriftung</t>
+        </is>
+      </c>
+      <c r="F101" t="inlineStr">
+        <is>
+          <t>rahmentuere_nebenraum_Typ1.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>2025-09-02T13:28:47</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>Haus_C.3dm</t>
+        </is>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>31d853aa-269c-46ac-b249-923c10675bd8</t>
+        </is>
+      </c>
+      <c r="D102" t="inlineStr">
+        <is>
+          <t>rahmentuere_w</t>
+        </is>
+      </c>
+      <c r="E102" t="inlineStr">
+        <is>
+          <t>Standard 1:10 Rahmenbeschriftung WHG Eingang</t>
+        </is>
+      </c>
+      <c r="F102" t="inlineStr">
+        <is>
+          <t>rahmentuerew.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>2025-09-02T13:38:03</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>Haus_C.3dm</t>
+        </is>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>f3eb2b1a-236c-4905-97e9-6861e8c8c8c8</t>
+        </is>
+      </c>
+      <c r="D103" t="inlineStr">
+        <is>
+          <t>zargentuere</t>
+        </is>
+      </c>
+      <c r="E103" t="inlineStr">
+        <is>
+          <t>Standard 1:10 Zargenbeschriftung</t>
+        </is>
+      </c>
+      <c r="F103" t="inlineStr">
+        <is>
+          <t>zargentuere.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>2025-09-02T13:39:08</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>Haus_C.3dm</t>
+        </is>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>628397d5-d3ed-4e4e-b29c-b03e38cb7220</t>
+        </is>
+      </c>
+      <c r="D104" t="inlineStr">
+        <is>
+          <t>zargentuere</t>
+        </is>
+      </c>
+      <c r="E104" t="inlineStr">
+        <is>
+          <t>Standard 1:10 Zargenbeschriftung</t>
+        </is>
+      </c>
+      <c r="F104" t="inlineStr">
+        <is>
+          <t>zargentuere.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>2025-09-02T13:39:48</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>Haus_C.3dm</t>
+        </is>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>100d485b-89d2-488c-8a11-7921512318a4</t>
+        </is>
+      </c>
+      <c r="D105" t="inlineStr">
+        <is>
+          <t>zargentuere</t>
+        </is>
+      </c>
+      <c r="E105" t="inlineStr">
+        <is>
+          <t>Standard 1:10 Zargenbeschriftung</t>
+        </is>
+      </c>
+      <c r="F105" t="inlineStr">
+        <is>
+          <t>zargentuere.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>2025-09-02T13:44:11</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>Haus_C.3dm</t>
+        </is>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>5f65a4ae-b45b-4dcc-bf4a-0f3298438b60</t>
+        </is>
+      </c>
+      <c r="D106" t="inlineStr">
+        <is>
+          <t>zargentuere</t>
+        </is>
+      </c>
+      <c r="E106" t="inlineStr">
+        <is>
+          <t>Standard 1:10 Zargenbeschriftung</t>
+        </is>
+      </c>
+      <c r="F106" t="inlineStr">
+        <is>
+          <t>zargentuere.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>2025-09-02T13:45:04</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>Haus_C.3dm</t>
+        </is>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>7c663c7d-cd63-47f0-b12d-131c37316bad</t>
+        </is>
+      </c>
+      <c r="D107" t="inlineStr">
+        <is>
+          <t>zargentuere</t>
+        </is>
+      </c>
+      <c r="E107" t="inlineStr">
+        <is>
+          <t>Standard 1:10 Zargenbeschriftung</t>
+        </is>
+      </c>
+      <c r="F107" t="inlineStr">
+        <is>
+          <t>zargentuere.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>2025-09-02T13:45:49</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>Haus_C.3dm</t>
+        </is>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>6c73ef6a-9911-4b34-a9fb-e848fa37826a</t>
+        </is>
+      </c>
+      <c r="D108" t="inlineStr">
+        <is>
+          <t>zargentuere</t>
+        </is>
+      </c>
+      <c r="E108" t="inlineStr">
+        <is>
+          <t>Standard 1:10 Zargenbeschriftung</t>
+        </is>
+      </c>
+      <c r="F108" t="inlineStr">
+        <is>
+          <t>zargentuere.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>2025-09-02T13:46:17</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>Haus_C.3dm</t>
+        </is>
+      </c>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>09e45927-87da-484a-bcd8-bdde1a385b57</t>
+        </is>
+      </c>
+      <c r="D109" t="inlineStr">
+        <is>
+          <t>rahmentuere_w</t>
+        </is>
+      </c>
+      <c r="E109" t="inlineStr">
+        <is>
+          <t>Standard 1:10 Rahmenbeschriftung WHG Eingang</t>
+        </is>
+      </c>
+      <c r="F109" t="inlineStr">
+        <is>
+          <t>rahmentuerew.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>2025-09-02T13:47:37</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>Haus_C.3dm</t>
+        </is>
+      </c>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>4f037136-281f-4b99-8589-be70fc04c301</t>
+        </is>
+      </c>
+      <c r="D110" t="inlineStr">
+        <is>
+          <t>zargentuere</t>
+        </is>
+      </c>
+      <c r="E110" t="inlineStr">
+        <is>
+          <t>Standard 1:10 Zargenbeschriftung</t>
+        </is>
+      </c>
+      <c r="F110" t="inlineStr">
+        <is>
+          <t>zargentuere.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>2025-09-02T13:48:16</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>Haus_C.3dm</t>
+        </is>
+      </c>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>cb9c2449-a120-4523-8594-3c503fbea85c</t>
+        </is>
+      </c>
+      <c r="D111" t="inlineStr">
+        <is>
+          <t>zargentuere</t>
+        </is>
+      </c>
+      <c r="E111" t="inlineStr">
+        <is>
+          <t>Standard 1:10 Zargenbeschriftung</t>
+        </is>
+      </c>
+      <c r="F111" t="inlineStr">
+        <is>
+          <t>zargentuere.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>2025-09-02T13:51:21</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>Haus_C.3dm</t>
+        </is>
+      </c>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>3d0d9ae1-0433-4a11-9aa8-97034d27e2c0</t>
+        </is>
+      </c>
+      <c r="D112" t="inlineStr">
+        <is>
+          <t>zargentuere</t>
+        </is>
+      </c>
+      <c r="E112" t="inlineStr">
+        <is>
+          <t>Standard 1:10 Zargenbeschriftung</t>
+        </is>
+      </c>
+      <c r="F112" t="inlineStr">
+        <is>
+          <t>zargentuere.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>2025-09-02T13:52:07</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>Haus_C.3dm</t>
+        </is>
+      </c>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t>baff48db-0cf8-4e7e-96d1-bc8808a68bb5</t>
+        </is>
+      </c>
+      <c r="D113" t="inlineStr">
+        <is>
+          <t>schiebetuere</t>
+        </is>
+      </c>
+      <c r="E113" t="inlineStr">
+        <is>
+          <t>Standard 1:10 Schiebetürbeschriftung</t>
+        </is>
+      </c>
+      <c r="F113" t="inlineStr">
+        <is>
+          <t>schiebetuere.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>2025-09-02T13:54:24</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>Haus_C.3dm</t>
+        </is>
+      </c>
+      <c r="C114" t="inlineStr">
+        <is>
+          <t>941c1c94-4f7f-47be-bfa1-9b77a0bbb557</t>
+        </is>
+      </c>
+      <c r="D114" t="inlineStr">
+        <is>
+          <t>rahmentuere_w</t>
+        </is>
+      </c>
+      <c r="E114" t="inlineStr">
+        <is>
+          <t>Standard 1:10 Rahmenbeschriftung WHG Eingang</t>
+        </is>
+      </c>
+      <c r="F114" t="inlineStr">
+        <is>
+          <t>rahmentuerew.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>2025-09-02T13:55:38</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>Haus_C.3dm</t>
+        </is>
+      </c>
+      <c r="C115" t="inlineStr">
+        <is>
+          <t>5bf2bff0-3ec4-4dfe-b37d-18ca1964a2e9</t>
+        </is>
+      </c>
+      <c r="D115" t="inlineStr">
+        <is>
+          <t>zargentuere</t>
+        </is>
+      </c>
+      <c r="E115" t="inlineStr">
+        <is>
+          <t>Standard 1:10 Zargenbeschriftung</t>
+        </is>
+      </c>
+      <c r="F115" t="inlineStr">
+        <is>
+          <t>zargentuere.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>2025-09-02T13:56:26</t>
+        </is>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>Haus_C.3dm</t>
+        </is>
+      </c>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>d9d92a28-99b9-41a4-affb-f7ff4a41dfd8</t>
+        </is>
+      </c>
+      <c r="D116" t="inlineStr">
+        <is>
+          <t>zargentuere</t>
+        </is>
+      </c>
+      <c r="E116" t="inlineStr">
+        <is>
+          <t>Standard 1:10 Zargenbeschriftung</t>
+        </is>
+      </c>
+      <c r="F116" t="inlineStr">
+        <is>
+          <t>zargentuere.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>2025-09-02T13:58:42</t>
+        </is>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>Haus_C.3dm</t>
+        </is>
+      </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>dea8b753-483a-467b-bf45-f8e8fff466d8</t>
+        </is>
+      </c>
+      <c r="D117" t="inlineStr">
+        <is>
+          <t>zargentuere</t>
+        </is>
+      </c>
+      <c r="E117" t="inlineStr">
+        <is>
+          <t>Standard 1:10 Zargenbeschriftung</t>
+        </is>
+      </c>
+      <c r="F117" t="inlineStr">
+        <is>
+          <t>zargentuere.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>2025-09-02T13:59:11</t>
+        </is>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>Haus_C.3dm</t>
+        </is>
+      </c>
+      <c r="C118" t="inlineStr">
+        <is>
+          <t>a8a51296-c90d-4f80-94b3-d6f990110ddd</t>
+        </is>
+      </c>
+      <c r="D118" t="inlineStr">
+        <is>
+          <t>zargentuere</t>
+        </is>
+      </c>
+      <c r="E118" t="inlineStr">
+        <is>
+          <t>Standard 1:10 Zargenbeschriftung</t>
+        </is>
+      </c>
+      <c r="F118" t="inlineStr">
+        <is>
+          <t>zargentuere.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>2025-09-02T14:00:02</t>
+        </is>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>Haus_C.3dm</t>
+        </is>
+      </c>
+      <c r="C119" t="inlineStr">
+        <is>
+          <t>c6fb5dea-2209-4155-8a5a-a3a56619748e</t>
+        </is>
+      </c>
+      <c r="D119" t="inlineStr">
+        <is>
+          <t>rahmentuere</t>
+        </is>
+      </c>
+      <c r="E119" t="inlineStr">
+        <is>
+          <t>Standard 1:10 Rahmenbeschriftung</t>
+        </is>
+      </c>
+      <c r="F119" t="inlineStr">
+        <is>
+          <t>rahmentuere_nebenraum_Typ1.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>2025-09-02T14:01:05</t>
+        </is>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>Haus_C.3dm</t>
+        </is>
+      </c>
+      <c r="C120" t="inlineStr">
+        <is>
+          <t>025714c3-0990-4516-bbe6-d62fb7ecaad2</t>
+        </is>
+      </c>
+      <c r="D120" t="inlineStr">
+        <is>
+          <t>rahmentuere_w</t>
+        </is>
+      </c>
+      <c r="E120" t="inlineStr">
+        <is>
+          <t>Standard 1:10 Rahmenbeschriftung WHG Eingang</t>
+        </is>
+      </c>
+      <c r="F120" t="inlineStr">
+        <is>
+          <t>rahmentuerew.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>2025-09-02T14:14:20</t>
+        </is>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>Haus_C.3dm</t>
+        </is>
+      </c>
+      <c r="C121" t="inlineStr">
+        <is>
+          <t>e8e034eb-8ff5-41cd-a69a-f75530fc26f7</t>
+        </is>
+      </c>
+      <c r="D121" t="inlineStr">
+        <is>
+          <t>zargentuere</t>
+        </is>
+      </c>
+      <c r="E121" t="inlineStr">
+        <is>
+          <t>Standard 1:10 Zargenbeschriftung</t>
+        </is>
+      </c>
+      <c r="F121" t="inlineStr">
+        <is>
+          <t>zargentuere.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>2025-09-02T14:18:59</t>
+        </is>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>Haus_C.3dm</t>
+        </is>
+      </c>
+      <c r="C122" t="inlineStr">
+        <is>
+          <t>24d327dc-f312-4b1e-b759-fa9ddcbce0cf</t>
+        </is>
+      </c>
+      <c r="D122" t="inlineStr">
+        <is>
+          <t>zargentuere</t>
+        </is>
+      </c>
+      <c r="E122" t="inlineStr">
+        <is>
+          <t>Standard 1:10 Zargenbeschriftung</t>
+        </is>
+      </c>
+      <c r="F122" t="inlineStr">
+        <is>
+          <t>zargentuere.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>2025-09-02T14:23:22</t>
+        </is>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>Haus_C.3dm</t>
+        </is>
+      </c>
+      <c r="C123" t="inlineStr">
+        <is>
+          <t>5e31b98f-f6b0-43ff-9528-ec4eb0663fdb</t>
+        </is>
+      </c>
+      <c r="D123" t="inlineStr">
+        <is>
+          <t>zargentuere</t>
+        </is>
+      </c>
+      <c r="E123" t="inlineStr">
+        <is>
+          <t>Standard 1:10 Zargenbeschriftung</t>
+        </is>
+      </c>
+      <c r="F123" t="inlineStr">
+        <is>
+          <t>zargentuere.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>2025-09-02T14:24:13</t>
+        </is>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>Haus_C.3dm</t>
+        </is>
+      </c>
+      <c r="C124" t="inlineStr">
+        <is>
+          <t>6705cba6-d6d7-4375-a7d3-f281c16d71b3</t>
+        </is>
+      </c>
+      <c r="D124" t="inlineStr">
+        <is>
+          <t>zargentuere</t>
+        </is>
+      </c>
+      <c r="E124" t="inlineStr">
+        <is>
+          <t>Standard 1:10 Zargenbeschriftung</t>
+        </is>
+      </c>
+      <c r="F124" t="inlineStr">
+        <is>
+          <t>zargentuere.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="inlineStr">
+        <is>
+          <t>2025-09-02T14:25:18</t>
+        </is>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>Haus_C.3dm</t>
+        </is>
+      </c>
+      <c r="C125" t="inlineStr">
+        <is>
+          <t>9675d0c4-a797-4a2a-8734-ce2b00d523b2</t>
+        </is>
+      </c>
+      <c r="D125" t="inlineStr">
+        <is>
+          <t>zargentuere</t>
+        </is>
+      </c>
+      <c r="E125" t="inlineStr">
+        <is>
+          <t>Standard 1:10 Zargenbeschriftung</t>
+        </is>
+      </c>
+      <c r="F125" t="inlineStr">
+        <is>
+          <t>zargentuere.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="inlineStr">
+        <is>
+          <t>2025-09-02T14:26:02</t>
+        </is>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>Haus_C.3dm</t>
+        </is>
+      </c>
+      <c r="C126" t="inlineStr">
+        <is>
+          <t>efcc8c45-8196-4a36-acd2-a4e225dadbdb</t>
+        </is>
+      </c>
+      <c r="D126" t="inlineStr">
+        <is>
+          <t>zargentuere</t>
+        </is>
+      </c>
+      <c r="E126" t="inlineStr">
+        <is>
+          <t>Standard 1:10 Zargenbeschriftung</t>
+        </is>
+      </c>
+      <c r="F126" t="inlineStr">
+        <is>
+          <t>zargentuere.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="inlineStr">
+        <is>
+          <t>2025-09-02T14:27:05</t>
+        </is>
+      </c>
+      <c r="B127" t="inlineStr">
+        <is>
+          <t>Haus_C.3dm</t>
+        </is>
+      </c>
+      <c r="C127" t="inlineStr">
+        <is>
+          <t>6a58b12d-7b1a-4b79-ae3f-b9ad378beadb</t>
+        </is>
+      </c>
+      <c r="D127" t="inlineStr">
+        <is>
+          <t>rahmentuere_w</t>
+        </is>
+      </c>
+      <c r="E127" t="inlineStr">
+        <is>
+          <t>Standard 1:10 Rahmenbeschriftung WHG Eingang</t>
+        </is>
+      </c>
+      <c r="F127" t="inlineStr">
+        <is>
+          <t>rahmentuerew.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="inlineStr">
+        <is>
+          <t>2025-09-02T14:28:11</t>
+        </is>
+      </c>
+      <c r="B128" t="inlineStr">
+        <is>
+          <t>Haus_C.3dm</t>
+        </is>
+      </c>
+      <c r="C128" t="inlineStr">
+        <is>
+          <t>16bf6ef4-520b-4b33-a080-247ff6b393f7</t>
+        </is>
+      </c>
+      <c r="D128" t="inlineStr">
+        <is>
+          <t>zargentuere</t>
+        </is>
+      </c>
+      <c r="E128" t="inlineStr">
+        <is>
+          <t>Standard 1:10 Zargenbeschriftung</t>
+        </is>
+      </c>
+      <c r="F128" t="inlineStr">
+        <is>
+          <t>zargentuere.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="inlineStr">
+        <is>
+          <t>2025-09-02T14:28:53</t>
+        </is>
+      </c>
+      <c r="B129" t="inlineStr">
+        <is>
+          <t>Haus_C.3dm</t>
+        </is>
+      </c>
+      <c r="C129" t="inlineStr">
+        <is>
+          <t>16b10756-a47b-4ccd-8ba3-a5b58f28cb29</t>
+        </is>
+      </c>
+      <c r="D129" t="inlineStr">
+        <is>
+          <t>zargentuere</t>
+        </is>
+      </c>
+      <c r="E129" t="inlineStr">
+        <is>
+          <t>Standard 1:10 Zargenbeschriftung</t>
+        </is>
+      </c>
+      <c r="F129" t="inlineStr">
+        <is>
+          <t>zargentuere.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="inlineStr">
+        <is>
+          <t>2025-09-02T14:30:23</t>
+        </is>
+      </c>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>Haus_C.3dm</t>
+        </is>
+      </c>
+      <c r="C130" t="inlineStr">
+        <is>
+          <t>a538d334-8ea9-49ce-adf0-2eb78da2c44e</t>
+        </is>
+      </c>
+      <c r="D130" t="inlineStr">
+        <is>
+          <t>zargentuere</t>
+        </is>
+      </c>
+      <c r="E130" t="inlineStr">
+        <is>
+          <t>Standard 1:10 Zargenbeschriftung</t>
+        </is>
+      </c>
+      <c r="F130" t="inlineStr">
+        <is>
+          <t>zargentuere.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="inlineStr">
+        <is>
+          <t>2025-09-02T14:31:15</t>
+        </is>
+      </c>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>Haus_C.3dm</t>
+        </is>
+      </c>
+      <c r="C131" t="inlineStr">
+        <is>
+          <t>4a4fe479-f5ff-40ac-94c5-f9122b2177d1</t>
+        </is>
+      </c>
+      <c r="D131" t="inlineStr">
+        <is>
+          <t>schiebetuere</t>
+        </is>
+      </c>
+      <c r="E131" t="inlineStr">
+        <is>
+          <t>Standard 1:10 Schiebetürbeschriftung</t>
+        </is>
+      </c>
+      <c r="F131" t="inlineStr">
+        <is>
+          <t>schiebetuere.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="inlineStr">
+        <is>
+          <t>2025-09-02T14:34:40</t>
+        </is>
+      </c>
+      <c r="B132" t="inlineStr">
+        <is>
+          <t>Haus_C.3dm</t>
+        </is>
+      </c>
+      <c r="C132" t="inlineStr">
+        <is>
+          <t>5783c73e-ba87-4989-9422-371a90149e14</t>
+        </is>
+      </c>
+      <c r="D132" t="inlineStr">
+        <is>
+          <t>rahmentuere_w</t>
+        </is>
+      </c>
+      <c r="E132" t="inlineStr">
+        <is>
+          <t>Standard 1:10 Rahmenbeschriftung WHG Eingang</t>
+        </is>
+      </c>
+      <c r="F132" t="inlineStr">
+        <is>
+          <t>rahmentuerew.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="inlineStr">
+        <is>
+          <t>2025-09-02T14:38:33</t>
+        </is>
+      </c>
+      <c r="B133" t="inlineStr">
+        <is>
+          <t>Haus_C.3dm</t>
+        </is>
+      </c>
+      <c r="C133" t="inlineStr">
+        <is>
+          <t>97c135d6-f88c-42ff-b230-6b11bd0bf614</t>
+        </is>
+      </c>
+      <c r="D133" t="inlineStr">
+        <is>
+          <t>zargentuere</t>
+        </is>
+      </c>
+      <c r="E133" t="inlineStr">
+        <is>
+          <t>Standard 1:10 Zargenbeschriftung</t>
+        </is>
+      </c>
+      <c r="F133" t="inlineStr">
+        <is>
+          <t>zargentuere_zimmer_M150.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="inlineStr">
+        <is>
+          <t>2025-09-02T14:39:02</t>
+        </is>
+      </c>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>Haus_C.3dm</t>
+        </is>
+      </c>
+      <c r="C134" t="inlineStr">
+        <is>
+          <t>4222e3dc-ddd4-43b4-a2be-578637260114</t>
+        </is>
+      </c>
+      <c r="D134" t="inlineStr">
+        <is>
+          <t>zargentuere</t>
+        </is>
+      </c>
+      <c r="E134" t="inlineStr">
+        <is>
+          <t>Standard 1:10 Zargenbeschriftung</t>
+        </is>
+      </c>
+      <c r="F134" t="inlineStr">
+        <is>
+          <t>zargentuere_zimmer_M150.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="inlineStr">
+        <is>
+          <t>2025-09-02T14:39:57</t>
+        </is>
+      </c>
+      <c r="B135" t="inlineStr">
+        <is>
+          <t>Haus_C.3dm</t>
+        </is>
+      </c>
+      <c r="C135" t="inlineStr">
+        <is>
+          <t>97bfd594-196f-4dac-b5ab-b57c5eed4741</t>
+        </is>
+      </c>
+      <c r="D135" t="inlineStr">
+        <is>
+          <t>zargentuere</t>
+        </is>
+      </c>
+      <c r="E135" t="inlineStr">
+        <is>
+          <t>Standard 1:10 Zargenbeschriftung</t>
+        </is>
+      </c>
+      <c r="F135" t="inlineStr">
+        <is>
+          <t>zargentuere_zimmer_M150.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="inlineStr">
+        <is>
+          <t>2025-09-02T14:40:23</t>
+        </is>
+      </c>
+      <c r="B136" t="inlineStr">
+        <is>
+          <t>Haus_C.3dm</t>
+        </is>
+      </c>
+      <c r="C136" t="inlineStr">
+        <is>
+          <t>58996c5a-ac97-4622-96b0-bdf27319f86e</t>
+        </is>
+      </c>
+      <c r="D136" t="inlineStr">
+        <is>
+          <t>rahmentuere</t>
+        </is>
+      </c>
+      <c r="E136" t="inlineStr">
+        <is>
+          <t>Standard 1:10 Rahmenbeschriftung</t>
+        </is>
+      </c>
+      <c r="F136" t="inlineStr">
+        <is>
+          <t>rahmentuere_nebenraum_Typ1.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="inlineStr">
+        <is>
+          <t>2025-09-02T14:43:25</t>
+        </is>
+      </c>
+      <c r="B137" t="inlineStr">
+        <is>
+          <t>Haus_C.3dm</t>
+        </is>
+      </c>
+      <c r="C137" t="inlineStr">
+        <is>
+          <t>873f66f0-87cf-4a1e-beb1-3a171cde36cb</t>
+        </is>
+      </c>
+      <c r="D137" t="inlineStr">
+        <is>
+          <t>zargentuere</t>
+        </is>
+      </c>
+      <c r="E137" t="inlineStr">
+        <is>
+          <t>Standard 1:10 Zargenbeschriftung</t>
+        </is>
+      </c>
+      <c r="F137" t="inlineStr">
+        <is>
+          <t>zargentuere_zimmer_M150.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="inlineStr">
+        <is>
+          <t>2025-09-02T14:43:57</t>
+        </is>
+      </c>
+      <c r="B138" t="inlineStr">
+        <is>
+          <t>Haus_C.3dm</t>
+        </is>
+      </c>
+      <c r="C138" t="inlineStr">
+        <is>
+          <t>8c4e6446-2e60-4346-b0a3-158c7d026615</t>
+        </is>
+      </c>
+      <c r="D138" t="inlineStr">
+        <is>
+          <t>rahmentuere_w</t>
+        </is>
+      </c>
+      <c r="E138" t="inlineStr">
+        <is>
+          <t>Standard 1:10 Rahmenbeschriftung WHG Eingang</t>
+        </is>
+      </c>
+      <c r="F138" t="inlineStr">
+        <is>
+          <t>rahmentuerew.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="inlineStr">
+        <is>
+          <t>2025-09-02T14:46:21</t>
+        </is>
+      </c>
+      <c r="B139" t="inlineStr">
+        <is>
+          <t>Haus_C.3dm</t>
+        </is>
+      </c>
+      <c r="C139" t="inlineStr">
+        <is>
+          <t>95345d17-95c6-44b4-846b-7fb06bb194ab</t>
+        </is>
+      </c>
+      <c r="D139" t="inlineStr">
+        <is>
+          <t>zargentuere</t>
+        </is>
+      </c>
+      <c r="E139" t="inlineStr">
+        <is>
+          <t>Standard 1:10 Zargenbeschriftung</t>
+        </is>
+      </c>
+      <c r="F139" t="inlineStr">
+        <is>
+          <t>zargentuere_zimmer_M120.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="inlineStr">
+        <is>
+          <t>2025-09-02T14:47:14</t>
+        </is>
+      </c>
+      <c r="B140" t="inlineStr">
+        <is>
+          <t>Haus_C.3dm</t>
+        </is>
+      </c>
+      <c r="C140" t="inlineStr">
+        <is>
+          <t>be85d00c-dce7-45a8-881b-aff397842b54</t>
+        </is>
+      </c>
+      <c r="D140" t="inlineStr">
+        <is>
+          <t>zargentuere</t>
+        </is>
+      </c>
+      <c r="E140" t="inlineStr">
+        <is>
+          <t>Standard 1:10 Zargenbeschriftung</t>
+        </is>
+      </c>
+      <c r="F140" t="inlineStr">
+        <is>
+          <t>zargentuere_zimmer_M150.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="inlineStr">
+        <is>
+          <t>2025-09-02T14:51:18</t>
+        </is>
+      </c>
+      <c r="B141" t="inlineStr">
+        <is>
+          <t>Haus_C.3dm</t>
+        </is>
+      </c>
+      <c r="C141" t="inlineStr">
+        <is>
+          <t>d8c31dde-289c-4bb0-a3dd-814e7c023800</t>
+        </is>
+      </c>
+      <c r="D141" t="inlineStr">
+        <is>
+          <t>zargentuere</t>
+        </is>
+      </c>
+      <c r="E141" t="inlineStr">
+        <is>
+          <t>Standard 1:10 Zargenbeschriftung</t>
+        </is>
+      </c>
+      <c r="F141" t="inlineStr">
+        <is>
+          <t>zargentuere_zimmer_M150.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="inlineStr">
+        <is>
+          <t>2025-09-02T14:52:07</t>
+        </is>
+      </c>
+      <c r="B142" t="inlineStr">
+        <is>
+          <t>Haus_C.3dm</t>
+        </is>
+      </c>
+      <c r="C142" t="inlineStr">
+        <is>
+          <t>07c60b59-6626-4df1-86cb-9150afaf4cd4</t>
+        </is>
+      </c>
+      <c r="D142" t="inlineStr">
+        <is>
+          <t>zargentuere</t>
+        </is>
+      </c>
+      <c r="E142" t="inlineStr">
+        <is>
+          <t>Standard 1:10 Zargenbeschriftung</t>
+        </is>
+      </c>
+      <c r="F142" t="inlineStr">
+        <is>
+          <t>zargentuere_zimmer_M150.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="inlineStr">
+        <is>
+          <t>2025-09-02T14:53:00</t>
+        </is>
+      </c>
+      <c r="B143" t="inlineStr">
+        <is>
+          <t>Haus_C.3dm</t>
+        </is>
+      </c>
+      <c r="C143" t="inlineStr">
+        <is>
+          <t>db22d5f0-32f4-4bd7-a95a-62e7ecb30b1b</t>
+        </is>
+      </c>
+      <c r="D143" t="inlineStr">
+        <is>
+          <t>rahmentuere_w</t>
+        </is>
+      </c>
+      <c r="E143" t="inlineStr">
+        <is>
+          <t>Standard 1:10 Rahmenbeschriftung WHG Eingang</t>
+        </is>
+      </c>
+      <c r="F143" t="inlineStr">
+        <is>
+          <t>rahmentuerew.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="inlineStr">
+        <is>
+          <t>2025-09-02T14:53:46</t>
+        </is>
+      </c>
+      <c r="B144" t="inlineStr">
+        <is>
+          <t>Haus_C.3dm</t>
+        </is>
+      </c>
+      <c r="C144" t="inlineStr">
+        <is>
+          <t>57a8057e-1873-4dab-82fd-c8fdcd363f22</t>
+        </is>
+      </c>
+      <c r="D144" t="inlineStr">
+        <is>
+          <t>zargentuere</t>
+        </is>
+      </c>
+      <c r="E144" t="inlineStr">
+        <is>
+          <t>Standard 1:10 Zargenbeschriftung</t>
+        </is>
+      </c>
+      <c r="F144" t="inlineStr">
+        <is>
+          <t>zargentuere.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="inlineStr">
+        <is>
+          <t>2025-09-02T14:54:39</t>
+        </is>
+      </c>
+      <c r="B145" t="inlineStr">
+        <is>
+          <t>Haus_C.3dm</t>
+        </is>
+      </c>
+      <c r="C145" t="inlineStr">
+        <is>
+          <t>632178a7-8bad-4c98-875f-290ab8ff1ad8</t>
+        </is>
+      </c>
+      <c r="D145" t="inlineStr">
+        <is>
+          <t>zargentuere</t>
+        </is>
+      </c>
+      <c r="E145" t="inlineStr">
+        <is>
+          <t>Standard 1:10 Zargenbeschriftung</t>
+        </is>
+      </c>
+      <c r="F145" t="inlineStr">
+        <is>
+          <t>zargentuere.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="inlineStr">
+        <is>
+          <t>2025-09-02T14:55:23</t>
+        </is>
+      </c>
+      <c r="B146" t="inlineStr">
+        <is>
+          <t>Haus_C.3dm</t>
+        </is>
+      </c>
+      <c r="C146" t="inlineStr">
+        <is>
+          <t>9eb37517-1009-45b3-a879-676b745a6c42</t>
+        </is>
+      </c>
+      <c r="D146" t="inlineStr">
+        <is>
+          <t>zargentuere</t>
+        </is>
+      </c>
+      <c r="E146" t="inlineStr">
+        <is>
+          <t>Standard 1:10 Zargenbeschriftung</t>
+        </is>
+      </c>
+      <c r="F146" t="inlineStr">
+        <is>
+          <t>zargentuere.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="inlineStr">
+        <is>
+          <t>2025-09-02T15:14:10</t>
+        </is>
+      </c>
+      <c r="B147" t="inlineStr">
+        <is>
+          <t>Haus_C.3dm</t>
+        </is>
+      </c>
+      <c r="C147" t="inlineStr">
+        <is>
+          <t>df3b15be-b84a-47a0-b7c8-3ec08dc9fb8f</t>
+        </is>
+      </c>
+      <c r="D147" t="inlineStr">
+        <is>
+          <t>schiebetuere</t>
+        </is>
+      </c>
+      <c r="E147" t="inlineStr">
+        <is>
+          <t>Standard 1:10 Schiebetürbeschriftung</t>
+        </is>
+      </c>
+      <c r="F147" t="inlineStr">
+        <is>
+          <t>schiebetuere.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="inlineStr">
+        <is>
+          <t>2025-09-02T15:15:02</t>
+        </is>
+      </c>
+      <c r="B148" t="inlineStr">
+        <is>
+          <t>Haus_C.3dm</t>
+        </is>
+      </c>
+      <c r="C148" t="inlineStr">
+        <is>
+          <t>767dcbef-f5d2-4bce-b673-d3b43846973b</t>
+        </is>
+      </c>
+      <c r="D148" t="inlineStr">
+        <is>
+          <t>schiebetuere</t>
+        </is>
+      </c>
+      <c r="E148" t="inlineStr">
+        <is>
+          <t>Standard 1:10 Schiebetürbeschriftung</t>
+        </is>
+      </c>
+      <c r="F148" t="inlineStr">
+        <is>
+          <t>schiebetuere.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="inlineStr">
+        <is>
+          <t>2025-09-02T15:16:35</t>
+        </is>
+      </c>
+      <c r="B149" t="inlineStr">
+        <is>
+          <t>Haus_C.3dm</t>
+        </is>
+      </c>
+      <c r="C149" t="inlineStr">
+        <is>
+          <t>9156e4d2-f97f-47f8-82fc-84e37341a398</t>
+        </is>
+      </c>
+      <c r="D149" t="inlineStr">
+        <is>
+          <t>rahmentuere_w</t>
+        </is>
+      </c>
+      <c r="E149" t="inlineStr">
+        <is>
+          <t>Standard 1:10 Rahmenbeschriftung WHG Eingang</t>
+        </is>
+      </c>
+      <c r="F149" t="inlineStr">
+        <is>
+          <t>rahmentuerew.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="inlineStr">
+        <is>
+          <t>2025-09-02T15:17:27</t>
+        </is>
+      </c>
+      <c r="B150" t="inlineStr">
+        <is>
+          <t>Haus_C.3dm</t>
+        </is>
+      </c>
+      <c r="C150" t="inlineStr">
+        <is>
+          <t>825e27fa-d279-408d-ba30-ce54bd777bba</t>
+        </is>
+      </c>
+      <c r="D150" t="inlineStr">
+        <is>
+          <t>zargentuere</t>
+        </is>
+      </c>
+      <c r="E150" t="inlineStr">
+        <is>
+          <t>Standard 1:10 Zargenbeschriftung</t>
+        </is>
+      </c>
+      <c r="F150" t="inlineStr">
+        <is>
+          <t>zargentuere_zimmer_M150.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="inlineStr">
+        <is>
+          <t>2025-09-02T15:17:55</t>
+        </is>
+      </c>
+      <c r="B151" t="inlineStr">
+        <is>
+          <t>Haus_C.3dm</t>
+        </is>
+      </c>
+      <c r="C151" t="inlineStr">
+        <is>
+          <t>0cb95c66-694a-4572-9980-3bb03c0e5dc3</t>
+        </is>
+      </c>
+      <c r="D151" t="inlineStr">
+        <is>
+          <t>zargentuere</t>
+        </is>
+      </c>
+      <c r="E151" t="inlineStr">
+        <is>
+          <t>Standard 1:10 Zargenbeschriftung</t>
+        </is>
+      </c>
+      <c r="F151" t="inlineStr">
+        <is>
+          <t>zargentuere_zimmer_M150.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="inlineStr">
+        <is>
+          <t>2025-09-02T15:23:44</t>
+        </is>
+      </c>
+      <c r="B152" t="inlineStr">
+        <is>
+          <t>Haus_C.3dm</t>
+        </is>
+      </c>
+      <c r="C152" t="inlineStr">
+        <is>
+          <t>3f671efd-9c34-4a9c-a01d-d2a5f6a2fae0</t>
+        </is>
+      </c>
+      <c r="D152" t="inlineStr">
+        <is>
+          <t>rahmentuere</t>
+        </is>
+      </c>
+      <c r="E152" t="inlineStr">
+        <is>
+          <t>Standard 1:10 Rahmenbeschriftung</t>
+        </is>
+      </c>
+      <c r="F152" t="inlineStr">
+        <is>
+          <t>rahmentuere_nebenraum_Typ1.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="inlineStr">
+        <is>
+          <t>2025-09-02T15:25:11</t>
+        </is>
+      </c>
+      <c r="B153" t="inlineStr">
+        <is>
+          <t>Haus_C.3dm</t>
+        </is>
+      </c>
+      <c r="C153" t="inlineStr">
+        <is>
+          <t>6b54247f-860a-4efc-b6a0-19dbb5279110</t>
+        </is>
+      </c>
+      <c r="D153" t="inlineStr">
+        <is>
+          <t>rahmentuere</t>
+        </is>
+      </c>
+      <c r="E153" t="inlineStr">
+        <is>
+          <t>Standard 1:10 Rahmenbeschriftung</t>
+        </is>
+      </c>
+      <c r="F153" t="inlineStr">
+        <is>
+          <t>rahmentuere_nebenraum_Typ1.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="inlineStr">
+        <is>
+          <t>2025-09-02T15:25:53</t>
+        </is>
+      </c>
+      <c r="B154" t="inlineStr">
+        <is>
+          <t>Haus_C.3dm</t>
+        </is>
+      </c>
+      <c r="C154" t="inlineStr">
+        <is>
+          <t>0d491230-4bda-499a-8604-f11dc6eb48e5</t>
+        </is>
+      </c>
+      <c r="D154" t="inlineStr">
+        <is>
+          <t>rahmentuere_w</t>
+        </is>
+      </c>
+      <c r="E154" t="inlineStr">
+        <is>
+          <t>Standard 1:10 Rahmenbeschriftung WHG Eingang</t>
+        </is>
+      </c>
+      <c r="F154" t="inlineStr">
+        <is>
+          <t>rahmentuerew.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="inlineStr">
+        <is>
+          <t>2025-09-02T15:27:34</t>
+        </is>
+      </c>
+      <c r="B155" t="inlineStr">
+        <is>
+          <t>Haus_C.3dm</t>
+        </is>
+      </c>
+      <c r="C155" t="inlineStr">
+        <is>
+          <t>030e3969-4d5d-4f27-80a9-ca51893a5f32</t>
+        </is>
+      </c>
+      <c r="D155" t="inlineStr">
+        <is>
+          <t>zargentuere</t>
+        </is>
+      </c>
+      <c r="E155" t="inlineStr">
+        <is>
+          <t>Standard 1:10 Zargenbeschriftung</t>
+        </is>
+      </c>
+      <c r="F155" t="inlineStr">
+        <is>
+          <t>zargentuere_zimmer_M150.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="inlineStr">
+        <is>
+          <t>2025-09-02T15:29:15</t>
+        </is>
+      </c>
+      <c r="B156" t="inlineStr">
+        <is>
+          <t>Haus_C.3dm</t>
+        </is>
+      </c>
+      <c r="C156" t="inlineStr">
+        <is>
+          <t>fd4d767f-b898-47d6-bda5-189ef691ff16</t>
+        </is>
+      </c>
+      <c r="D156" t="inlineStr">
+        <is>
+          <t>zargentuere</t>
+        </is>
+      </c>
+      <c r="E156" t="inlineStr">
+        <is>
+          <t>Standard 1:10 Zargenbeschriftung</t>
+        </is>
+      </c>
+      <c r="F156" t="inlineStr">
+        <is>
+          <t>zargentuere_zimmer_M150.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="inlineStr">
+        <is>
+          <t>2025-09-02T15:29:44</t>
+        </is>
+      </c>
+      <c r="B157" t="inlineStr">
+        <is>
+          <t>Haus_C.3dm</t>
+        </is>
+      </c>
+      <c r="C157" t="inlineStr">
+        <is>
+          <t>1e69977b-7c20-426a-94bf-1df377735adc</t>
+        </is>
+      </c>
+      <c r="D157" t="inlineStr">
+        <is>
+          <t>schiebetuere</t>
+        </is>
+      </c>
+      <c r="E157" t="inlineStr">
+        <is>
+          <t>Standard 1:10 Schiebetürbeschriftung</t>
+        </is>
+      </c>
+      <c r="F157" t="inlineStr">
+        <is>
+          <t>schiebetuere.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="inlineStr">
+        <is>
+          <t>2025-09-02T15:30:18</t>
+        </is>
+      </c>
+      <c r="B158" t="inlineStr">
+        <is>
+          <t>Haus_C.3dm</t>
+        </is>
+      </c>
+      <c r="C158" t="inlineStr">
+        <is>
+          <t>6f8b3b50-8d19-4219-82fc-4984b5e11938</t>
+        </is>
+      </c>
+      <c r="D158" t="inlineStr">
+        <is>
+          <t>zargentuere</t>
+        </is>
+      </c>
+      <c r="E158" t="inlineStr">
+        <is>
+          <t>Standard 1:10 Zargenbeschriftung</t>
+        </is>
+      </c>
+      <c r="F158" t="inlineStr">
+        <is>
+          <t>zargentuere_zimmer_M150.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="inlineStr">
+        <is>
+          <t>2025-09-02T15:30:42</t>
+        </is>
+      </c>
+      <c r="B159" t="inlineStr">
+        <is>
+          <t>Haus_C.3dm</t>
+        </is>
+      </c>
+      <c r="C159" t="inlineStr">
+        <is>
+          <t>38d73505-9b2e-4b69-a5d4-7d41ebe503b0</t>
+        </is>
+      </c>
+      <c r="D159" t="inlineStr">
+        <is>
+          <t>schiebetuere</t>
+        </is>
+      </c>
+      <c r="E159" t="inlineStr">
+        <is>
+          <t>Standard 1:10 Schiebetürbeschriftung</t>
+        </is>
+      </c>
+      <c r="F159" t="inlineStr">
+        <is>
+          <t>schiebetuere.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="inlineStr">
+        <is>
+          <t>2025-09-02T15:31:37</t>
+        </is>
+      </c>
+      <c r="B160" t="inlineStr">
+        <is>
+          <t>Haus_C.3dm</t>
+        </is>
+      </c>
+      <c r="C160" t="inlineStr">
+        <is>
+          <t>8b812c9a-374d-4740-98f0-a4f8c386bdac</t>
+        </is>
+      </c>
+      <c r="D160" t="inlineStr">
+        <is>
+          <t>zargentuere</t>
+        </is>
+      </c>
+      <c r="E160" t="inlineStr">
+        <is>
+          <t>Standard 1:10 Zargenbeschriftung</t>
+        </is>
+      </c>
+      <c r="F160" t="inlineStr">
+        <is>
+          <t>zargentuere_zimmer_M150.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="inlineStr">
+        <is>
+          <t>2025-09-02T15:32:00</t>
+        </is>
+      </c>
+      <c r="B161" t="inlineStr">
+        <is>
+          <t>Haus_C.3dm</t>
+        </is>
+      </c>
+      <c r="C161" t="inlineStr">
+        <is>
+          <t>fc3b2806-9ba9-4a14-9f6b-bf7d27d4dfd4</t>
+        </is>
+      </c>
+      <c r="D161" t="inlineStr">
+        <is>
+          <t>zargentuere</t>
+        </is>
+      </c>
+      <c r="E161" t="inlineStr">
+        <is>
+          <t>Standard 1:10 Zargenbeschriftung</t>
+        </is>
+      </c>
+      <c r="F161" t="inlineStr">
+        <is>
+          <t>zargentuere_zimmer_M150.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="inlineStr">
+        <is>
+          <t>2025-09-02T15:32:47</t>
+        </is>
+      </c>
+      <c r="B162" t="inlineStr">
+        <is>
+          <t>Haus_C.3dm</t>
+        </is>
+      </c>
+      <c r="C162" t="inlineStr">
+        <is>
+          <t>b930dba4-919b-4adc-967f-acba9d5801ef</t>
+        </is>
+      </c>
+      <c r="D162" t="inlineStr">
+        <is>
+          <t>zargentuere</t>
+        </is>
+      </c>
+      <c r="E162" t="inlineStr">
+        <is>
+          <t>Standard 1:10 Zargenbeschriftung</t>
+        </is>
+      </c>
+      <c r="F162" t="inlineStr">
+        <is>
+          <t>zargentuere_zimmer_M150.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="inlineStr">
+        <is>
+          <t>2025-09-02T15:33:55</t>
+        </is>
+      </c>
+      <c r="B163" t="inlineStr">
+        <is>
+          <t>Haus_C.3dm</t>
+        </is>
+      </c>
+      <c r="C163" t="inlineStr">
+        <is>
+          <t>50bb9596-d44c-4a4f-8b62-804f405e23a2</t>
+        </is>
+      </c>
+      <c r="D163" t="inlineStr">
+        <is>
+          <t>rahmentuere_w</t>
+        </is>
+      </c>
+      <c r="E163" t="inlineStr">
+        <is>
+          <t>Standard 1:10 Rahmenbeschriftung WHG Eingang</t>
+        </is>
+      </c>
+      <c r="F163" t="inlineStr">
+        <is>
+          <t>rahmentuerew.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="inlineStr">
+        <is>
+          <t>2025-09-02T15:34:52</t>
+        </is>
+      </c>
+      <c r="B164" t="inlineStr">
+        <is>
+          <t>Haus_C.3dm</t>
+        </is>
+      </c>
+      <c r="C164" t="inlineStr">
+        <is>
+          <t>c4d6879c-ce83-422d-b1bb-2c643235f4e8</t>
+        </is>
+      </c>
+      <c r="D164" t="inlineStr">
+        <is>
+          <t>zargentuere</t>
+        </is>
+      </c>
+      <c r="E164" t="inlineStr">
+        <is>
+          <t>Standard 1:10 Zargenbeschriftung</t>
+        </is>
+      </c>
+      <c r="F164" t="inlineStr">
+        <is>
+          <t>zargentuere_zimmer_M150.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="inlineStr">
+        <is>
+          <t>2025-09-02T15:36:29</t>
+        </is>
+      </c>
+      <c r="B165" t="inlineStr">
+        <is>
+          <t>Haus_C.3dm</t>
+        </is>
+      </c>
+      <c r="C165" t="inlineStr">
+        <is>
+          <t>17b5fff8-7616-4c4f-ae77-f38d7dd08fd5</t>
+        </is>
+      </c>
+      <c r="D165" t="inlineStr">
+        <is>
+          <t>schiebetuere</t>
+        </is>
+      </c>
+      <c r="E165" t="inlineStr">
+        <is>
+          <t>Standard 1:10 Schiebetürbeschriftung</t>
+        </is>
+      </c>
+      <c r="F165" t="inlineStr">
+        <is>
+          <t>schiebetuere.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="inlineStr">
+        <is>
+          <t>2025-09-02T15:37:12</t>
+        </is>
+      </c>
+      <c r="B166" t="inlineStr">
+        <is>
+          <t>Haus_C.3dm</t>
+        </is>
+      </c>
+      <c r="C166" t="inlineStr">
+        <is>
+          <t>f8d81720-3522-4a19-873e-d39219ce309c</t>
+        </is>
+      </c>
+      <c r="D166" t="inlineStr">
+        <is>
+          <t>zargentuere</t>
+        </is>
+      </c>
+      <c r="E166" t="inlineStr">
+        <is>
+          <t>Standard 1:10 Zargenbeschriftung</t>
+        </is>
+      </c>
+      <c r="F166" t="inlineStr">
+        <is>
+          <t>zargentuere_zimmer_M120.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="inlineStr">
+        <is>
+          <t>2025-09-02T15:38:15</t>
+        </is>
+      </c>
+      <c r="B167" t="inlineStr">
+        <is>
+          <t>Haus_C.3dm</t>
+        </is>
+      </c>
+      <c r="C167" t="inlineStr">
+        <is>
+          <t>06736e49-73de-4864-a844-e2856a7a6990</t>
+        </is>
+      </c>
+      <c r="D167" t="inlineStr">
+        <is>
+          <t>schiebetuere</t>
+        </is>
+      </c>
+      <c r="E167" t="inlineStr">
+        <is>
+          <t>Standard 1:10 Schiebetürbeschriftung</t>
+        </is>
+      </c>
+      <c r="F167" t="inlineStr">
+        <is>
+          <t>schiebetuere.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="inlineStr">
+        <is>
+          <t>2025-09-02T15:39:21</t>
+        </is>
+      </c>
+      <c r="B168" t="inlineStr">
+        <is>
+          <t>Haus_C.3dm</t>
+        </is>
+      </c>
+      <c r="C168" t="inlineStr">
+        <is>
+          <t>4a5e3da5-a0d5-4ce4-9318-ae6e5427c88a</t>
+        </is>
+      </c>
+      <c r="D168" t="inlineStr">
+        <is>
+          <t>zargentuere</t>
+        </is>
+      </c>
+      <c r="E168" t="inlineStr">
+        <is>
+          <t>Standard 1:10 Zargenbeschriftung</t>
+        </is>
+      </c>
+      <c r="F168" t="inlineStr">
+        <is>
+          <t>zargentuere_zimmer_M150.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="inlineStr">
+        <is>
+          <t>2025-09-02T15:39:54</t>
+        </is>
+      </c>
+      <c r="B169" t="inlineStr">
+        <is>
+          <t>Haus_C.3dm</t>
+        </is>
+      </c>
+      <c r="C169" t="inlineStr">
+        <is>
+          <t>53c2c021-f074-4457-b7c4-ba48623bdd49</t>
+        </is>
+      </c>
+      <c r="D169" t="inlineStr">
+        <is>
+          <t>spez</t>
+        </is>
+      </c>
+      <c r="E169" t="inlineStr">
+        <is>
+          <t>Standard 1:10 Spez.Rahmenbeschriftung</t>
+        </is>
+      </c>
+      <c r="F169" t="inlineStr">
+        <is>
+          <t>spez.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="inlineStr">
+        <is>
+          <t>2025-09-02T15:40:42</t>
+        </is>
+      </c>
+      <c r="B170" t="inlineStr">
+        <is>
+          <t>Haus_C.3dm</t>
+        </is>
+      </c>
+      <c r="C170" t="inlineStr">
+        <is>
+          <t>4e6b456e-56d7-413b-a91c-515e292d90e8</t>
+        </is>
+      </c>
+      <c r="D170" t="inlineStr">
+        <is>
+          <t>spez</t>
+        </is>
+      </c>
+      <c r="E170" t="inlineStr">
+        <is>
+          <t>Standard 1:10 Spez.Rahmenbeschriftung</t>
+        </is>
+      </c>
+      <c r="F170" t="inlineStr">
+        <is>
+          <t>spez.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="inlineStr">
+        <is>
+          <t>2025-09-02T15:41:04</t>
+        </is>
+      </c>
+      <c r="B171" t="inlineStr">
+        <is>
+          <t>Haus_C.3dm</t>
+        </is>
+      </c>
+      <c r="C171" t="inlineStr">
+        <is>
+          <t>b91ba800-8bb2-4b48-ab27-ee8779ec3e1e</t>
+        </is>
+      </c>
+      <c r="D171" t="inlineStr">
+        <is>
+          <t>spez</t>
+        </is>
+      </c>
+      <c r="E171" t="inlineStr">
+        <is>
+          <t>Standard 1:10 Spez.Rahmenbeschriftung</t>
+        </is>
+      </c>
+      <c r="F171" t="inlineStr">
+        <is>
+          <t>spez.csv</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
neue Funktionen, ETO Dialog für den Export
</commit_message>
<xml_diff>
--- a/created_leaders_log.xlsx
+++ b/created_leaders_log.xlsx
@@ -322,7 +322,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F185"/>
+  <dimension ref="A1:F188"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6170,40 +6170,133 @@
       </c>
     </row>
     <row r="185" ht="15.75" customHeight="1" s="3">
-      <c r="A185" t="inlineStr">
+      <c r="A185" s="0" t="inlineStr">
         <is>
           <t>2025-10-02T11:13:40</t>
         </is>
       </c>
-      <c r="B185" t="inlineStr">
+      <c r="B185" s="0" t="inlineStr">
         <is>
           <t>Untitled</t>
         </is>
       </c>
-      <c r="C185" t="inlineStr">
+      <c r="C185" s="0" t="inlineStr">
         <is>
           <t>adc4bc2c-2271-4337-bbd4-2d764b166bb4</t>
         </is>
       </c>
-      <c r="D185" t="inlineStr">
+      <c r="D185" s="0" t="inlineStr">
         <is>
           <t>schiebetuere</t>
         </is>
       </c>
-      <c r="E185" t="inlineStr">
+      <c r="E185" s="0" t="inlineStr">
         <is>
           <t>Standard 1:10 Schiebetürbeschriftung</t>
         </is>
       </c>
-      <c r="F185" t="inlineStr">
+      <c r="F185" s="0" t="inlineStr">
         <is>
           <t>schiebetuere.csv</t>
         </is>
       </c>
     </row>
-    <row r="186" ht="15.75" customHeight="1" s="3"/>
-    <row r="187" ht="15.75" customHeight="1" s="3"/>
-    <row r="188" ht="15.75" customHeight="1" s="3"/>
+    <row r="186" ht="15.75" customHeight="1" s="3">
+      <c r="A186" s="0" t="inlineStr">
+        <is>
+          <t>2025-10-02T11:28:41</t>
+        </is>
+      </c>
+      <c r="B186" s="0" t="inlineStr">
+        <is>
+          <t>Untitled</t>
+        </is>
+      </c>
+      <c r="C186" s="0" t="inlineStr">
+        <is>
+          <t>37aed359-c26a-4879-a3b0-be72d0102e6c</t>
+        </is>
+      </c>
+      <c r="D186" s="0" t="inlineStr">
+        <is>
+          <t>zargentuere</t>
+        </is>
+      </c>
+      <c r="E186" s="0" t="inlineStr">
+        <is>
+          <t>Standard 1:10 Zargenbeschriftung</t>
+        </is>
+      </c>
+      <c r="F186" s="0" t="inlineStr">
+        <is>
+          <t>zargentuere_zimmer_M150.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="187" ht="15.75" customHeight="1" s="3">
+      <c r="A187" s="0" t="inlineStr">
+        <is>
+          <t>2025-10-02T13:23:55</t>
+        </is>
+      </c>
+      <c r="B187" s="0" t="inlineStr">
+        <is>
+          <t>Haus_A.3dm</t>
+        </is>
+      </c>
+      <c r="C187" s="0" t="inlineStr">
+        <is>
+          <t>902cfd9e-9c4e-43ed-a10e-439db871fb13</t>
+        </is>
+      </c>
+      <c r="D187" s="0" t="inlineStr">
+        <is>
+          <t>schiebetuere</t>
+        </is>
+      </c>
+      <c r="E187" s="0" t="inlineStr">
+        <is>
+          <t>Standard 1:10 Schiebetürbeschriftung</t>
+        </is>
+      </c>
+      <c r="F187" s="0" t="inlineStr">
+        <is>
+          <t>schiebetuere.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="188" ht="15.75" customHeight="1" s="3">
+      <c r="A188" t="inlineStr">
+        <is>
+          <t>2025-10-02T15:18:23</t>
+        </is>
+      </c>
+      <c r="B188" t="inlineStr">
+        <is>
+          <t>Haus_A.3dm</t>
+        </is>
+      </c>
+      <c r="C188" t="inlineStr">
+        <is>
+          <t>f6f1031a-2245-4d3d-9f7c-9d911d750bbb</t>
+        </is>
+      </c>
+      <c r="D188" t="inlineStr">
+        <is>
+          <t>schiebetuere</t>
+        </is>
+      </c>
+      <c r="E188" t="inlineStr">
+        <is>
+          <t>Standard 1:10 Schiebetürbeschriftung</t>
+        </is>
+      </c>
+      <c r="F188" t="inlineStr">
+        <is>
+          <t>schiebetuere.csv</t>
+        </is>
+      </c>
+    </row>
     <row r="189" ht="15.75" customHeight="1" s="3"/>
     <row r="190" ht="15.75" customHeight="1" s="3"/>
     <row r="191" ht="15.75" customHeight="1" s="3"/>

</xml_diff>

<commit_message>
Neues csv Template -> Schild Rosette Drücker hinzugefügt
</commit_message>
<xml_diff>
--- a/created_leaders_log.xlsx
+++ b/created_leaders_log.xlsx
@@ -322,7 +322,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F208"/>
+  <dimension ref="A1:F216"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6906,45 +6906,293 @@
       </c>
     </row>
     <row r="208" ht="15.75" customHeight="1" s="3">
-      <c r="A208" t="inlineStr">
+      <c r="A208" s="0" t="inlineStr">
         <is>
           <t>2025-10-07T06:36:21</t>
         </is>
       </c>
-      <c r="B208" t="inlineStr">
+      <c r="B208" s="0" t="inlineStr">
         <is>
           <t>25.0803_Akon_Dermanence_Grundriss.3dm</t>
         </is>
       </c>
-      <c r="C208" t="inlineStr">
+      <c r="C208" s="0" t="inlineStr">
         <is>
           <t>dedfa747-6a0e-4011-a6a8-21802d47d3ad</t>
         </is>
       </c>
-      <c r="D208" t="inlineStr">
-        <is>
-          <t>zargentuere</t>
-        </is>
-      </c>
-      <c r="E208" t="inlineStr">
-        <is>
-          <t>Standard 1:10 Zargenbeschriftung</t>
-        </is>
-      </c>
-      <c r="F208" t="inlineStr">
+      <c r="D208" s="0" t="inlineStr">
+        <is>
+          <t>zargentuere</t>
+        </is>
+      </c>
+      <c r="E208" s="0" t="inlineStr">
+        <is>
+          <t>Standard 1:10 Zargenbeschriftung</t>
+        </is>
+      </c>
+      <c r="F208" s="0" t="inlineStr">
         <is>
           <t>zargentuere_zimmer_M220_LBW_Furniert.csv</t>
         </is>
       </c>
     </row>
-    <row r="209" ht="15.75" customHeight="1" s="3"/>
-    <row r="210" ht="15.75" customHeight="1" s="3"/>
-    <row r="211" ht="15.75" customHeight="1" s="3"/>
-    <row r="212" ht="15.75" customHeight="1" s="3"/>
-    <row r="213" ht="15.75" customHeight="1" s="3"/>
-    <row r="214" ht="15.75" customHeight="1" s="3"/>
-    <row r="215" ht="15.75" customHeight="1" s="3"/>
-    <row r="216" ht="15.75" customHeight="1" s="3"/>
+    <row r="209" ht="15.75" customHeight="1" s="3">
+      <c r="A209" s="0" t="inlineStr">
+        <is>
+          <t>2025-10-14T16:59:53</t>
+        </is>
+      </c>
+      <c r="B209" s="0" t="inlineStr">
+        <is>
+          <t>25.0803_Akon_Dermanence_Grundrissneu_ab_dwg.3dm</t>
+        </is>
+      </c>
+      <c r="C209" s="0" t="inlineStr">
+        <is>
+          <t>bbf7e392-3a37-4155-b244-b1382392e1d0</t>
+        </is>
+      </c>
+      <c r="D209" s="0" t="inlineStr">
+        <is>
+          <t>schiebetuere</t>
+        </is>
+      </c>
+      <c r="E209" s="0" t="inlineStr">
+        <is>
+          <t>Standard 1:10 Schiebetürbeschriftung</t>
+        </is>
+      </c>
+      <c r="F209" s="0" t="inlineStr">
+        <is>
+          <t>schiebetuere.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="210" ht="15.75" customHeight="1" s="3">
+      <c r="A210" s="0" t="inlineStr">
+        <is>
+          <t>2025-10-16T09:33:05</t>
+        </is>
+      </c>
+      <c r="B210" s="0" t="inlineStr">
+        <is>
+          <t>Untitled</t>
+        </is>
+      </c>
+      <c r="C210" s="0" t="inlineStr">
+        <is>
+          <t>5f187c27-5d2a-4f8f-9ac3-288c2cbbe980</t>
+        </is>
+      </c>
+      <c r="D210" s="0" t="inlineStr">
+        <is>
+          <t>rahmentuere</t>
+        </is>
+      </c>
+      <c r="E210" s="0" t="inlineStr">
+        <is>
+          <t>Standard 1:10 Rahmenbeschriftung</t>
+        </is>
+      </c>
+      <c r="F210" s="0" t="inlineStr">
+        <is>
+          <t>rahmentuere.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="211" ht="15.75" customHeight="1" s="3">
+      <c r="A211" s="0" t="inlineStr">
+        <is>
+          <t>2025-10-16T09:33:34</t>
+        </is>
+      </c>
+      <c r="B211" s="0" t="inlineStr">
+        <is>
+          <t>Untitled</t>
+        </is>
+      </c>
+      <c r="C211" s="0" t="inlineStr">
+        <is>
+          <t>8a4bf1bf-617c-42a6-8cc3-a45bdc7d3eb6</t>
+        </is>
+      </c>
+      <c r="D211" s="0" t="inlineStr">
+        <is>
+          <t>rahmentuere</t>
+        </is>
+      </c>
+      <c r="E211" s="0" t="inlineStr">
+        <is>
+          <t>Standard 1:10 Rahmenbeschriftung</t>
+        </is>
+      </c>
+      <c r="F211" s="0" t="inlineStr">
+        <is>
+          <t>rahmentuere.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="212" ht="15.75" customHeight="1" s="3">
+      <c r="A212" s="0" t="inlineStr">
+        <is>
+          <t>2025-10-16T09:36:20</t>
+        </is>
+      </c>
+      <c r="B212" s="0" t="inlineStr">
+        <is>
+          <t>Untitled</t>
+        </is>
+      </c>
+      <c r="C212" s="0" t="inlineStr">
+        <is>
+          <t>986f81b8-ab95-4f8b-8a90-e8004634d8d2</t>
+        </is>
+      </c>
+      <c r="D212" s="0" t="inlineStr">
+        <is>
+          <t>rahmentuere</t>
+        </is>
+      </c>
+      <c r="E212" s="0" t="inlineStr">
+        <is>
+          <t>Standard 1:10 Rahmenbeschriftung</t>
+        </is>
+      </c>
+      <c r="F212" s="0" t="inlineStr">
+        <is>
+          <t>rahmentuere.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="213" ht="15.75" customHeight="1" s="3">
+      <c r="A213" s="0" t="inlineStr">
+        <is>
+          <t>2025-10-16T09:36:36</t>
+        </is>
+      </c>
+      <c r="B213" s="0" t="inlineStr">
+        <is>
+          <t>Untitled</t>
+        </is>
+      </c>
+      <c r="C213" s="0" t="inlineStr">
+        <is>
+          <t>7c73a897-bb99-457f-97d1-b3483bc29f2a</t>
+        </is>
+      </c>
+      <c r="D213" s="0" t="inlineStr">
+        <is>
+          <t>rahmentuere</t>
+        </is>
+      </c>
+      <c r="E213" s="0" t="inlineStr">
+        <is>
+          <t>Standard 1:10 Rahmenbeschriftung</t>
+        </is>
+      </c>
+      <c r="F213" s="0" t="inlineStr">
+        <is>
+          <t>rahmentuere.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="214" ht="15.75" customHeight="1" s="3">
+      <c r="A214" s="0" t="inlineStr">
+        <is>
+          <t>2025-10-16T09:36:57</t>
+        </is>
+      </c>
+      <c r="B214" s="0" t="inlineStr">
+        <is>
+          <t>Untitled</t>
+        </is>
+      </c>
+      <c r="C214" s="0" t="inlineStr">
+        <is>
+          <t>0ce0b9b6-3457-4d1b-aabc-a99c490daff3</t>
+        </is>
+      </c>
+      <c r="D214" s="0" t="inlineStr">
+        <is>
+          <t>rahmentuere</t>
+        </is>
+      </c>
+      <c r="E214" s="0" t="inlineStr">
+        <is>
+          <t>Standard 1:10 Rahmenbeschriftung</t>
+        </is>
+      </c>
+      <c r="F214" s="0" t="inlineStr">
+        <is>
+          <t>rahmentuere.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="215" ht="15.75" customHeight="1" s="3">
+      <c r="A215" s="0" t="inlineStr">
+        <is>
+          <t>2025-10-16T09:37:20</t>
+        </is>
+      </c>
+      <c r="B215" s="0" t="inlineStr">
+        <is>
+          <t>Untitled</t>
+        </is>
+      </c>
+      <c r="C215" s="0" t="inlineStr">
+        <is>
+          <t>2bdc1dc8-b6ee-4642-b318-ffd17e70545e</t>
+        </is>
+      </c>
+      <c r="D215" s="0" t="inlineStr">
+        <is>
+          <t>rahmentuere</t>
+        </is>
+      </c>
+      <c r="E215" s="0" t="inlineStr">
+        <is>
+          <t>Standard 1:10 Rahmenbeschriftung</t>
+        </is>
+      </c>
+      <c r="F215" s="0" t="inlineStr">
+        <is>
+          <t>rahmentuere.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="216" ht="15.75" customHeight="1" s="3">
+      <c r="A216" t="inlineStr">
+        <is>
+          <t>2025-10-16T09:37:35</t>
+        </is>
+      </c>
+      <c r="B216" t="inlineStr">
+        <is>
+          <t>Untitled</t>
+        </is>
+      </c>
+      <c r="C216" t="inlineStr">
+        <is>
+          <t>f6f1397b-917d-4dc7-b4ff-6e5329e2330c</t>
+        </is>
+      </c>
+      <c r="D216" t="inlineStr">
+        <is>
+          <t>rahmentuere</t>
+        </is>
+      </c>
+      <c r="E216" t="inlineStr">
+        <is>
+          <t>Standard 1:10 Rahmenbeschriftung</t>
+        </is>
+      </c>
+      <c r="F216" t="inlineStr">
+        <is>
+          <t>rahmentuere.csv</t>
+        </is>
+      </c>
+    </row>
     <row r="217" ht="15.75" customHeight="1" s="3"/>
     <row r="218" ht="15.75" customHeight="1" s="3"/>
     <row r="219" ht="15.75" customHeight="1" s="3"/>

</xml_diff>

<commit_message>
CSV angepasst, neues File
</commit_message>
<xml_diff>
--- a/created_leaders_log.xlsx
+++ b/created_leaders_log.xlsx
@@ -322,7 +322,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F216"/>
+  <dimension ref="A1:F223"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7162,44 +7162,261 @@
       </c>
     </row>
     <row r="216" ht="15.75" customHeight="1" s="3">
-      <c r="A216" t="inlineStr">
+      <c r="A216" s="0" t="inlineStr">
         <is>
           <t>2025-10-16T09:37:35</t>
         </is>
       </c>
-      <c r="B216" t="inlineStr">
+      <c r="B216" s="0" t="inlineStr">
         <is>
           <t>Untitled</t>
         </is>
       </c>
-      <c r="C216" t="inlineStr">
+      <c r="C216" s="0" t="inlineStr">
         <is>
           <t>f6f1397b-917d-4dc7-b4ff-6e5329e2330c</t>
         </is>
       </c>
-      <c r="D216" t="inlineStr">
+      <c r="D216" s="0" t="inlineStr">
         <is>
           <t>rahmentuere</t>
         </is>
       </c>
-      <c r="E216" t="inlineStr">
+      <c r="E216" s="0" t="inlineStr">
         <is>
           <t>Standard 1:10 Rahmenbeschriftung</t>
         </is>
       </c>
-      <c r="F216" t="inlineStr">
+      <c r="F216" s="0" t="inlineStr">
         <is>
           <t>rahmentuere.csv</t>
         </is>
       </c>
     </row>
-    <row r="217" ht="15.75" customHeight="1" s="3"/>
-    <row r="218" ht="15.75" customHeight="1" s="3"/>
-    <row r="219" ht="15.75" customHeight="1" s="3"/>
-    <row r="220" ht="15.75" customHeight="1" s="3"/>
-    <row r="221" ht="15.75" customHeight="1" s="3"/>
-    <row r="222" ht="15.75" customHeight="1" s="3"/>
-    <row r="223" ht="15.75" customHeight="1" s="3"/>
+    <row r="217" ht="15.75" customHeight="1" s="3">
+      <c r="A217" s="0" t="inlineStr">
+        <is>
+          <t>2025-10-16T10:33:57</t>
+        </is>
+      </c>
+      <c r="B217" s="0" t="inlineStr">
+        <is>
+          <t>Untitled</t>
+        </is>
+      </c>
+      <c r="C217" s="0" t="inlineStr">
+        <is>
+          <t>efa63824-f019-405b-b75a-639ac869047c</t>
+        </is>
+      </c>
+      <c r="D217" s="0" t="inlineStr">
+        <is>
+          <t>rahmentuere</t>
+        </is>
+      </c>
+      <c r="E217" s="0" t="inlineStr">
+        <is>
+          <t>Standard 1:10 Rahmenbeschriftung</t>
+        </is>
+      </c>
+      <c r="F217" s="0" t="inlineStr">
+        <is>
+          <t>rahmentuereBlockrahmen.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="218" ht="15.75" customHeight="1" s="3">
+      <c r="A218" s="0" t="inlineStr">
+        <is>
+          <t>2025-10-16T10:39:26</t>
+        </is>
+      </c>
+      <c r="B218" s="0" t="inlineStr">
+        <is>
+          <t>Untitled</t>
+        </is>
+      </c>
+      <c r="C218" s="0" t="inlineStr">
+        <is>
+          <t>94f76575-f7e5-441e-be91-ef4476f6181d</t>
+        </is>
+      </c>
+      <c r="D218" s="0" t="inlineStr">
+        <is>
+          <t>rahmentuere</t>
+        </is>
+      </c>
+      <c r="E218" s="0" t="inlineStr">
+        <is>
+          <t>Standard 1:10 Rahmenbeschriftung</t>
+        </is>
+      </c>
+      <c r="F218" s="0" t="inlineStr">
+        <is>
+          <t>rahmentuereBlockrahmen.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="219" ht="15.75" customHeight="1" s="3">
+      <c r="A219" s="0" t="inlineStr">
+        <is>
+          <t>2025-10-16T10:42:11</t>
+        </is>
+      </c>
+      <c r="B219" s="0" t="inlineStr">
+        <is>
+          <t>Untitled</t>
+        </is>
+      </c>
+      <c r="C219" s="0" t="inlineStr">
+        <is>
+          <t>c0d59d16-dda2-4acb-b083-f2b17560a1b2</t>
+        </is>
+      </c>
+      <c r="D219" s="0" t="inlineStr">
+        <is>
+          <t>rahmentuere</t>
+        </is>
+      </c>
+      <c r="E219" s="0" t="inlineStr">
+        <is>
+          <t>Standard 1:10 Rahmenbeschriftung</t>
+        </is>
+      </c>
+      <c r="F219" s="0" t="inlineStr">
+        <is>
+          <t>rahmentuereBlockrahmen.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="220" ht="15.75" customHeight="1" s="3">
+      <c r="A220" s="0" t="inlineStr">
+        <is>
+          <t>2025-10-16T10:42:50</t>
+        </is>
+      </c>
+      <c r="B220" s="0" t="inlineStr">
+        <is>
+          <t>Untitled</t>
+        </is>
+      </c>
+      <c r="C220" s="0" t="inlineStr">
+        <is>
+          <t>6894475a-8d1e-4644-a7eb-8938855707da</t>
+        </is>
+      </c>
+      <c r="D220" s="0" t="inlineStr">
+        <is>
+          <t>rahmentuere</t>
+        </is>
+      </c>
+      <c r="E220" s="0" t="inlineStr">
+        <is>
+          <t>Standard 1:10 Rahmenbeschriftung</t>
+        </is>
+      </c>
+      <c r="F220" s="0" t="inlineStr">
+        <is>
+          <t>rahmentuereBlockrahmen.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="221" ht="15.75" customHeight="1" s="3">
+      <c r="A221" s="0" t="inlineStr">
+        <is>
+          <t>2025-10-16T10:43:19</t>
+        </is>
+      </c>
+      <c r="B221" s="0" t="inlineStr">
+        <is>
+          <t>Untitled</t>
+        </is>
+      </c>
+      <c r="C221" s="0" t="inlineStr">
+        <is>
+          <t>f3c95967-ae33-496d-b12d-497bebd44286</t>
+        </is>
+      </c>
+      <c r="D221" s="0" t="inlineStr">
+        <is>
+          <t>rahmentuere</t>
+        </is>
+      </c>
+      <c r="E221" s="0" t="inlineStr">
+        <is>
+          <t>Standard 1:10 Rahmenbeschriftung</t>
+        </is>
+      </c>
+      <c r="F221" s="0" t="inlineStr">
+        <is>
+          <t>rahmentuereBlockrahmen.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="222" ht="15.75" customHeight="1" s="3">
+      <c r="A222" s="0" t="inlineStr">
+        <is>
+          <t>2025-10-16T10:43:34</t>
+        </is>
+      </c>
+      <c r="B222" s="0" t="inlineStr">
+        <is>
+          <t>Untitled</t>
+        </is>
+      </c>
+      <c r="C222" s="0" t="inlineStr">
+        <is>
+          <t>726ab9d8-5e81-44bd-bd0a-6e489a846532</t>
+        </is>
+      </c>
+      <c r="D222" s="0" t="inlineStr">
+        <is>
+          <t>rahmentuere</t>
+        </is>
+      </c>
+      <c r="E222" s="0" t="inlineStr">
+        <is>
+          <t>Standard 1:10 Rahmenbeschriftung</t>
+        </is>
+      </c>
+      <c r="F222" s="0" t="inlineStr">
+        <is>
+          <t>rahmentuereBlockrahmen.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="223" ht="15.75" customHeight="1" s="3">
+      <c r="A223" t="inlineStr">
+        <is>
+          <t>2025-10-16T10:43:52</t>
+        </is>
+      </c>
+      <c r="B223" t="inlineStr">
+        <is>
+          <t>Untitled</t>
+        </is>
+      </c>
+      <c r="C223" t="inlineStr">
+        <is>
+          <t>c881a14f-457d-43ea-bf8e-505042d6be41</t>
+        </is>
+      </c>
+      <c r="D223" t="inlineStr">
+        <is>
+          <t>rahmentuere</t>
+        </is>
+      </c>
+      <c r="E223" t="inlineStr">
+        <is>
+          <t>Standard 1:10 Rahmenbeschriftung</t>
+        </is>
+      </c>
+      <c r="F223" t="inlineStr">
+        <is>
+          <t>rahmentuereBlockrahmen.csv</t>
+        </is>
+      </c>
+    </row>
     <row r="224" ht="15.75" customHeight="1" s="3"/>
     <row r="225" ht="15.75" customHeight="1" s="3"/>
     <row r="226" ht="15.75" customHeight="1" s="3"/>

</xml_diff>